<commit_message>
Get weather strategy has been changed
</commit_message>
<xml_diff>
--- a/Weather/bin/Debug/netcoreapp3.1/output.xlsx
+++ b/Weather/bin/Debug/netcoreapp3.1/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -29,328 +29,325 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Vojens</t>
+    <t>Spennymoor</t>
+  </si>
+  <si>
+    <t>scattered clouds</t>
+  </si>
+  <si>
+    <t>Onga</t>
   </si>
   <si>
     <t>broken clouds</t>
   </si>
   <si>
-    <t>Argentona</t>
-  </si>
-  <si>
-    <t>Pedrosillo el Ralo</t>
+    <t>Great Barton</t>
   </si>
   <si>
     <t>few clouds</t>
   </si>
   <si>
-    <t>San Diego</t>
+    <t>Roussy-le-Village</t>
+  </si>
+  <si>
+    <t>light rain</t>
+  </si>
+  <si>
+    <t>Matraville</t>
   </si>
   <si>
     <t>clear sky</t>
   </si>
   <si>
-    <t>Wilrijk</t>
-  </si>
-  <si>
-    <t>Löffingen</t>
-  </si>
-  <si>
-    <t>Walnut Grove</t>
-  </si>
-  <si>
-    <t>Radnor</t>
-  </si>
-  <si>
-    <t>Kagawa</t>
-  </si>
-  <si>
-    <t>Maastricht</t>
+    <t>Mangaratiba</t>
+  </si>
+  <si>
+    <t>Perleberg</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Orgueil</t>
+  </si>
+  <si>
+    <t>Leopoldsdorf</t>
+  </si>
+  <si>
+    <t>Maysel</t>
   </si>
   <si>
     <t>overcast clouds</t>
   </si>
   <si>
-    <t>Klein Ammensleben</t>
-  </si>
-  <si>
-    <t>Paimio</t>
-  </si>
-  <si>
-    <t>Torbay</t>
-  </si>
-  <si>
-    <t>fog</t>
-  </si>
-  <si>
-    <t>Sérigné</t>
-  </si>
-  <si>
-    <t>Maple Shade Township</t>
-  </si>
-  <si>
-    <t>Neutraubling</t>
-  </si>
-  <si>
-    <t>Joane</t>
-  </si>
-  <si>
-    <t>Transinne</t>
-  </si>
-  <si>
-    <t>Venteuil</t>
-  </si>
-  <si>
-    <t>Coussay-les-Bois</t>
-  </si>
-  <si>
-    <t>Komotini</t>
-  </si>
-  <si>
-    <t>Essenheim</t>
-  </si>
-  <si>
-    <t>Niederdorf</t>
-  </si>
-  <si>
-    <t>scattered clouds</t>
-  </si>
-  <si>
-    <t>Courçon</t>
-  </si>
-  <si>
-    <t>Cuisery</t>
-  </si>
-  <si>
-    <t>Folcroft</t>
-  </si>
-  <si>
-    <t>Rountzenheim</t>
-  </si>
-  <si>
-    <t>Tekamah</t>
-  </si>
-  <si>
-    <t>mist</t>
-  </si>
-  <si>
-    <t>Boucau</t>
-  </si>
-  <si>
-    <t>Ault</t>
-  </si>
-  <si>
-    <t>Loire-sur-Rhône</t>
-  </si>
-  <si>
-    <t>Orbis</t>
-  </si>
-  <si>
-    <t>Houlle</t>
-  </si>
-  <si>
-    <t>light rain</t>
-  </si>
-  <si>
-    <t>Arrondissement de Bernay</t>
-  </si>
-  <si>
-    <t>Mníšek pod Brdy</t>
-  </si>
-  <si>
-    <t>Port Leyden</t>
-  </si>
-  <si>
-    <t>Penney Farms</t>
-  </si>
-  <si>
-    <t>Valleyview</t>
-  </si>
-  <si>
-    <t>Moussy</t>
-  </si>
-  <si>
-    <t>Kvidinge</t>
-  </si>
-  <si>
-    <t>Trierweiler</t>
-  </si>
-  <si>
-    <t>Miranda</t>
-  </si>
-  <si>
-    <t>Granollers</t>
-  </si>
-  <si>
-    <t>Long Branch</t>
-  </si>
-  <si>
-    <t>Wyocena</t>
-  </si>
-  <si>
-    <t>Lautenbach</t>
-  </si>
-  <si>
-    <t>Beachmere</t>
-  </si>
-  <si>
-    <t>Filo</t>
-  </si>
-  <si>
-    <t>Makkoshotyka</t>
-  </si>
-  <si>
-    <t>Otwock</t>
-  </si>
-  <si>
-    <t>Busto Garolfo</t>
-  </si>
-  <si>
-    <t>Bobingen</t>
-  </si>
-  <si>
-    <t>Ashford</t>
-  </si>
-  <si>
-    <t>Crick</t>
-  </si>
-  <si>
-    <t>Agoncillo</t>
-  </si>
-  <si>
-    <t>West Alexandria</t>
-  </si>
-  <si>
-    <t>Almada</t>
-  </si>
-  <si>
-    <t>Kottagūdem</t>
-  </si>
-  <si>
-    <t>Renedo</t>
-  </si>
-  <si>
-    <t>Bienenbüttel</t>
-  </si>
-  <si>
-    <t>Pervomayskaya</t>
-  </si>
-  <si>
-    <t>Hernshaw</t>
-  </si>
-  <si>
-    <t>The Dalles</t>
-  </si>
-  <si>
-    <t>Umuarama</t>
-  </si>
-  <si>
-    <t>Boothbay Harbor</t>
-  </si>
-  <si>
-    <t>Schwerstedt</t>
-  </si>
-  <si>
-    <t>Roggel</t>
-  </si>
-  <si>
-    <t>Chanteloup-les-Vignes</t>
-  </si>
-  <si>
-    <t>Le Mayet</t>
-  </si>
-  <si>
-    <t>Yakumo</t>
-  </si>
-  <si>
-    <t>Sloansville</t>
-  </si>
-  <si>
-    <t>Quixeramobim</t>
-  </si>
-  <si>
-    <t>Spanish Fork</t>
-  </si>
-  <si>
-    <t>Saint-Brisson-sur-Loire</t>
-  </si>
-  <si>
-    <t>Glenbeulah</t>
-  </si>
-  <si>
-    <t>Mangaratiba</t>
-  </si>
-  <si>
-    <t>Bassu</t>
-  </si>
-  <si>
-    <t>Villers-sur-Semois</t>
-  </si>
-  <si>
-    <t>Temerluh</t>
-  </si>
-  <si>
-    <t>Rejowiec</t>
-  </si>
-  <si>
-    <t>Le Pellerin</t>
-  </si>
-  <si>
-    <t>Salvirola</t>
-  </si>
-  <si>
-    <t>Zelhem</t>
-  </si>
-  <si>
-    <t>Bemelen</t>
-  </si>
-  <si>
-    <t>Tekoh</t>
-  </si>
-  <si>
-    <t>Vetren</t>
-  </si>
-  <si>
-    <t>Idaho Springs</t>
-  </si>
-  <si>
-    <t>Batavia</t>
-  </si>
-  <si>
-    <t>New Orleans</t>
-  </si>
-  <si>
-    <t>Marklohe</t>
-  </si>
-  <si>
-    <t>Couloisy</t>
-  </si>
-  <si>
-    <t>Lägerdorf</t>
-  </si>
-  <si>
-    <t>Pesqueira</t>
-  </si>
-  <si>
-    <t>DeMossville</t>
-  </si>
-  <si>
-    <t>Rozgarty</t>
-  </si>
-  <si>
-    <t>Hirakata</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
-  </si>
-  <si>
-    <t>Soe</t>
-  </si>
-  <si>
-    <t>Kempen</t>
-  </si>
-  <si>
-    <t>Aying</t>
+    <t>Brix</t>
+  </si>
+  <si>
+    <t>Picuí</t>
+  </si>
+  <si>
+    <t>Katonah</t>
+  </si>
+  <si>
+    <t>Gardelegen</t>
+  </si>
+  <si>
+    <t>Leonard</t>
+  </si>
+  <si>
+    <t>Geervliet</t>
+  </si>
+  <si>
+    <t>Sermoyer</t>
+  </si>
+  <si>
+    <t>Matawan</t>
+  </si>
+  <si>
+    <t>Baulkham Hills</t>
+  </si>
+  <si>
+    <t>Dmitrov</t>
+  </si>
+  <si>
+    <t>West Wyalong</t>
+  </si>
+  <si>
+    <t>Ravensburg</t>
+  </si>
+  <si>
+    <t>Boé</t>
+  </si>
+  <si>
+    <t>Dalhousie</t>
+  </si>
+  <si>
+    <t>Berric</t>
+  </si>
+  <si>
+    <t>Ocean Gate</t>
+  </si>
+  <si>
+    <t>Èze</t>
+  </si>
+  <si>
+    <t>Zheleznogorsk-Ilimskiy</t>
+  </si>
+  <si>
+    <t>Ondo</t>
+  </si>
+  <si>
+    <t>moderate rain</t>
+  </si>
+  <si>
+    <t>Desbiens</t>
+  </si>
+  <si>
+    <t>Novotroitsk</t>
+  </si>
+  <si>
+    <t>Saint-Jeures</t>
+  </si>
+  <si>
+    <t>Croughton</t>
+  </si>
+  <si>
+    <t>Holbæk</t>
+  </si>
+  <si>
+    <t>Dubach</t>
+  </si>
+  <si>
+    <t>Grobbendonk</t>
+  </si>
+  <si>
+    <t>Nagold</t>
+  </si>
+  <si>
+    <t>Graçay</t>
+  </si>
+  <si>
+    <t>Stanground</t>
+  </si>
+  <si>
+    <t>Engelsbrand</t>
+  </si>
+  <si>
+    <t>Saint-Antonin-sur-Bayon</t>
+  </si>
+  <si>
+    <t>Pampatar</t>
+  </si>
+  <si>
+    <t>Grainau</t>
+  </si>
+  <si>
+    <t>Cap-Santé</t>
+  </si>
+  <si>
+    <t>Manziat</t>
+  </si>
+  <si>
+    <t>Froggatt</t>
+  </si>
+  <si>
+    <t>Greytown</t>
+  </si>
+  <si>
+    <t>Torpes</t>
+  </si>
+  <si>
+    <t>Vamberk</t>
+  </si>
+  <si>
+    <t>Charron</t>
+  </si>
+  <si>
+    <t>Hammaslahti</t>
+  </si>
+  <si>
+    <t>Carol Stream</t>
+  </si>
+  <si>
+    <t>Ekkattuthangal</t>
+  </si>
+  <si>
+    <t>Saulieu</t>
+  </si>
+  <si>
+    <t>Fort Drum</t>
+  </si>
+  <si>
+    <t>Legemeer</t>
+  </si>
+  <si>
+    <t>Port-des-Barques</t>
+  </si>
+  <si>
+    <t>Osterberg</t>
+  </si>
+  <si>
+    <t>Estevelles</t>
+  </si>
+  <si>
+    <t>Seroa</t>
+  </si>
+  <si>
+    <t>Hartley</t>
+  </si>
+  <si>
+    <t>Courfaivre</t>
+  </si>
+  <si>
+    <t>Plaquemine</t>
+  </si>
+  <si>
+    <t>Frontera</t>
+  </si>
+  <si>
+    <t>Tocumbo</t>
+  </si>
+  <si>
+    <t>Jiangkou</t>
+  </si>
+  <si>
+    <t>Lake Jackson</t>
+  </si>
+  <si>
+    <t>Arrondissement de Saverne</t>
+  </si>
+  <si>
+    <t>Berwick</t>
+  </si>
+  <si>
+    <t>Cahul</t>
+  </si>
+  <si>
+    <t>Norges-la-Ville</t>
+  </si>
+  <si>
+    <t>Pirassununga</t>
+  </si>
+  <si>
+    <t>Valladolid</t>
+  </si>
+  <si>
+    <t>New Columbia</t>
+  </si>
+  <si>
+    <t>Masaki</t>
+  </si>
+  <si>
+    <t>Mellieħa</t>
+  </si>
+  <si>
+    <t>Ma’an</t>
+  </si>
+  <si>
+    <t>Klam</t>
+  </si>
+  <si>
+    <t>Stará Paka</t>
+  </si>
+  <si>
+    <t>Meillonnas</t>
+  </si>
+  <si>
+    <t>Schardenberg</t>
+  </si>
+  <si>
+    <t>Marienrachdorf</t>
+  </si>
+  <si>
+    <t>Modderfontein</t>
+  </si>
+  <si>
+    <t>Northborough</t>
+  </si>
+  <si>
+    <t>Sainte-Honorine-du-Fay</t>
+  </si>
+  <si>
+    <t>Polgár</t>
+  </si>
+  <si>
+    <t>Reynosa</t>
+  </si>
+  <si>
+    <t>Jessheim</t>
+  </si>
+  <si>
+    <t>Téglás</t>
+  </si>
+  <si>
+    <t>Mosnang</t>
+  </si>
+  <si>
+    <t>Fresnes-sur-Escaut</t>
+  </si>
+  <si>
+    <t>Bam</t>
+  </si>
+  <si>
+    <t>Gamaches</t>
+  </si>
+  <si>
+    <t>Guyong</t>
+  </si>
+  <si>
+    <t>Quint-Fonsegrives</t>
+  </si>
+  <si>
+    <t>Boulieu-lès-Annonay</t>
+  </si>
+  <si>
+    <t>Lake Geneva</t>
+  </si>
+  <si>
+    <t>Wegberg</t>
+  </si>
+  <si>
+    <t>Głubczyce</t>
   </si>
 </sst>
 </file>
@@ -417,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.81020164489746" customWidth="1"/>
+    <col min="1" max="1" width="25.70026969909668" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="11.25179672241211" customWidth="1"/>
     <col min="4" max="4" width="11.688645362854004" customWidth="1"/>
@@ -446,13 +443,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="0">
-        <v>15.260000228881836</v>
+        <v>13.140000343322754</v>
       </c>
       <c r="C2" s="0">
-        <v>1011</v>
+        <v>992</v>
       </c>
       <c r="D2" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>6</v>
@@ -463,373 +460,373 @@
         <v>7</v>
       </c>
       <c r="B3" s="0">
-        <v>23.25</v>
+        <v>14.359999656677246</v>
       </c>
       <c r="C3" s="0">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="D3" s="0">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0">
-        <v>19.81999969482422</v>
+        <v>15.420000076293945</v>
       </c>
       <c r="C4" s="0">
-        <v>1022</v>
+        <v>999</v>
       </c>
       <c r="D4" s="0">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0">
-        <v>18.15999984741211</v>
+        <v>14.279999732971191</v>
       </c>
       <c r="C5" s="0">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="D5" s="0">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0">
-        <v>16.239999771118164</v>
+        <v>16.799999237060547</v>
       </c>
       <c r="C6" s="0">
-        <v>1013</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0">
-        <v>18.469999313354492</v>
+        <v>34.47999954223633</v>
       </c>
       <c r="C7" s="0">
-        <v>1017</v>
+        <v>1009</v>
       </c>
       <c r="D7" s="0">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0">
-        <v>10.010000228881836</v>
+        <v>18.420000076293945</v>
       </c>
       <c r="C8" s="0">
-        <v>1025</v>
+        <v>1006</v>
       </c>
       <c r="D8" s="0">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0">
-        <v>13.140000343322754</v>
+        <v>9.010000228881836</v>
       </c>
       <c r="C9" s="0">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D9" s="0">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0">
-        <v>20.469999313354492</v>
+        <v>13.800000190734863</v>
       </c>
       <c r="C10" s="0">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="D10" s="0">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0">
-        <v>17.799999237060547</v>
+        <v>21.170000076293945</v>
       </c>
       <c r="C11" s="0">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D11" s="0">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0">
-        <v>19.639999389648438</v>
+        <v>14.800000190734863</v>
       </c>
       <c r="C12" s="0">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="D12" s="0">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0">
-        <v>12.3100004196167</v>
+        <v>14.960000038146973</v>
       </c>
       <c r="C13" s="0">
-        <v>1023</v>
+        <v>1005</v>
       </c>
       <c r="D13" s="0">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0">
-        <v>16.139999389648438</v>
+        <v>33.84000015258789</v>
       </c>
       <c r="C14" s="0">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="D14" s="0">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0">
-        <v>17.1200008392334</v>
+        <v>22.079999923706055</v>
       </c>
       <c r="C15" s="0">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="D15" s="0">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="0">
-        <v>13.890000343322754</v>
+        <v>19.809999465942383</v>
       </c>
       <c r="C16" s="0">
-        <v>1026</v>
+        <v>1005</v>
       </c>
       <c r="D16" s="0">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="0">
-        <v>18.290000915527344</v>
+        <v>25.639999389648438</v>
       </c>
       <c r="C17" s="0">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D17" s="0">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0">
-        <v>22.209999084472656</v>
+        <v>13.399999618530273</v>
       </c>
       <c r="C18" s="0">
-        <v>1021</v>
+        <v>1001</v>
       </c>
       <c r="D18" s="0">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0">
-        <v>14.479999542236328</v>
+        <v>14.100000381469727</v>
       </c>
       <c r="C19" s="0">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D19" s="0">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0">
-        <v>16.989999771118164</v>
+        <v>23.950000762939453</v>
       </c>
       <c r="C20" s="0">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D20" s="0">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0">
-        <v>16.309999465942383</v>
+        <v>16.559999465942383</v>
       </c>
       <c r="C21" s="0">
-        <v>1017</v>
+        <v>998</v>
       </c>
       <c r="D21" s="0">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0">
-        <v>21.75</v>
+        <v>8.359999656677246</v>
       </c>
       <c r="C22" s="0">
-        <v>1023</v>
+        <v>1034</v>
       </c>
       <c r="D22" s="0">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0">
-        <v>18.229999542236328</v>
+        <v>12.15999984741211</v>
       </c>
       <c r="C23" s="0">
-        <v>1016</v>
+        <v>1000</v>
       </c>
       <c r="D23" s="0">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0">
-        <v>17</v>
+        <v>21.1200008392334</v>
       </c>
       <c r="C24" s="0">
-        <v>1019</v>
+        <v>1008</v>
       </c>
       <c r="D24" s="0">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -837,16 +834,16 @@
         <v>34</v>
       </c>
       <c r="B25" s="0">
-        <v>17.81999969482422</v>
+        <v>15.079999923706055</v>
       </c>
       <c r="C25" s="0">
-        <v>1018</v>
+        <v>1013</v>
       </c>
       <c r="D25" s="0">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
@@ -854,16 +851,16 @@
         <v>35</v>
       </c>
       <c r="B26" s="0">
-        <v>20.530000686645508</v>
+        <v>14.0600004196167</v>
       </c>
       <c r="C26" s="0">
-        <v>1017</v>
+        <v>1009</v>
       </c>
       <c r="D26" s="0">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27">
@@ -871,16 +868,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="0">
-        <v>14.079999923706055</v>
+        <v>16.290000915527344</v>
       </c>
       <c r="C27" s="0">
-        <v>1026</v>
+        <v>1009</v>
       </c>
       <c r="D27" s="0">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -888,16 +885,16 @@
         <v>37</v>
       </c>
       <c r="B28" s="0">
-        <v>19.950000762939453</v>
+        <v>23.959999084472656</v>
       </c>
       <c r="C28" s="0">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="D28" s="0">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
@@ -905,50 +902,50 @@
         <v>38</v>
       </c>
       <c r="B29" s="0">
-        <v>18.940000534057617</v>
+        <v>20.420000076293945</v>
       </c>
       <c r="C29" s="0">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="D29" s="0">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="0">
-        <v>20.1299991607666</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C30" s="0">
-        <v>1020</v>
+        <v>1031</v>
       </c>
       <c r="D30" s="0">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="C31" s="0">
+        <v>1009</v>
+      </c>
+      <c r="D31" s="0">
+        <v>88</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B31" s="0">
-        <v>14.960000038146973</v>
-      </c>
-      <c r="C31" s="0">
-        <v>1012</v>
-      </c>
-      <c r="D31" s="0">
-        <v>90</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="32">
@@ -956,13 +953,13 @@
         <v>42</v>
       </c>
       <c r="B32" s="0">
-        <v>23.520000457763672</v>
+        <v>11.359999656677246</v>
       </c>
       <c r="C32" s="0">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D32" s="0">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>6</v>
@@ -973,16 +970,16 @@
         <v>43</v>
       </c>
       <c r="B33" s="0">
-        <v>17.809999465942383</v>
+        <v>7.389999866485596</v>
       </c>
       <c r="C33" s="0">
-        <v>1017</v>
+        <v>1030</v>
       </c>
       <c r="D33" s="0">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34">
@@ -990,608 +987,608 @@
         <v>44</v>
       </c>
       <c r="B34" s="0">
-        <v>14.470000267028809</v>
+        <v>9.890000343322754</v>
       </c>
       <c r="C34" s="0">
         <v>1011</v>
       </c>
       <c r="D34" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="0">
-        <v>15.079999923706055</v>
+        <v>13.5</v>
       </c>
       <c r="C35" s="0">
-        <v>1013</v>
+        <v>999</v>
       </c>
       <c r="D35" s="0">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="0">
-        <v>17.799999237060547</v>
+        <v>16.15999984741211</v>
       </c>
       <c r="C36" s="0">
-        <v>1020</v>
+        <v>998</v>
       </c>
       <c r="D36" s="0">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0">
-        <v>9.5</v>
+        <v>23.579999923706055</v>
       </c>
       <c r="C37" s="0">
-        <v>1024</v>
+        <v>1016</v>
       </c>
       <c r="D37" s="0">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="0">
-        <v>25.719999313354492</v>
+        <v>12.720000267028809</v>
       </c>
       <c r="C38" s="0">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="D38" s="0">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="0">
-        <v>4.019999980926514</v>
+        <v>18.6200008392334</v>
       </c>
       <c r="C39" s="0">
-        <v>1019</v>
+        <v>1009</v>
       </c>
       <c r="D39" s="0">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="0">
-        <v>17.549999237060547</v>
+        <v>14.609999656677246</v>
       </c>
       <c r="C40" s="0">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="D40" s="0">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="0">
-        <v>14.300000190734863</v>
+        <v>15.430000305175781</v>
       </c>
       <c r="C41" s="0">
-        <v>1016</v>
+        <v>996</v>
       </c>
       <c r="D41" s="0">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="0">
-        <v>17.149999618530273</v>
+        <v>15.699999809265137</v>
       </c>
       <c r="C42" s="0">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="D42" s="0">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="0">
-        <v>21.06999969482422</v>
+        <v>20.329999923706055</v>
       </c>
       <c r="C43" s="0">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="D43" s="0">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="0">
-        <v>23.18000030517578</v>
+        <v>36.029998779296875</v>
       </c>
       <c r="C44" s="0">
-        <v>1019</v>
+        <v>1011</v>
       </c>
       <c r="D44" s="0">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="0">
-        <v>14.770000457763672</v>
+        <v>19.329999923706055</v>
       </c>
       <c r="C45" s="0">
-        <v>1023</v>
+        <v>1010</v>
       </c>
       <c r="D45" s="0">
         <v>69</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="0">
-        <v>15.5600004196167</v>
+        <v>13.90999984741211</v>
       </c>
       <c r="C46" s="0">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="D46" s="0">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="0">
-        <v>19.809999465942383</v>
+        <v>14.130000114440918</v>
       </c>
       <c r="C47" s="0">
-        <v>1018</v>
+        <v>1011</v>
       </c>
       <c r="D47" s="0">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="0">
-        <v>14.84000015258789</v>
+        <v>13.420000076293945</v>
       </c>
       <c r="C48" s="0">
-        <v>1007</v>
+        <v>995</v>
       </c>
       <c r="D48" s="0">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="0">
-        <v>22.579999923706055</v>
+        <v>9.050000190734863</v>
       </c>
       <c r="C49" s="0">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D49" s="0">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="0">
-        <v>14.300000190734863</v>
+        <v>14.40999984741211</v>
       </c>
       <c r="C50" s="0">
-        <v>1027</v>
+        <v>1011</v>
       </c>
       <c r="D50" s="0">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="0">
-        <v>15.180000305175781</v>
+        <v>16.889999389648438</v>
       </c>
       <c r="C51" s="0">
-        <v>1026</v>
+        <v>1011</v>
       </c>
       <c r="D51" s="0">
         <v>70</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="0">
-        <v>20.950000762939453</v>
+        <v>18.010000228881836</v>
       </c>
       <c r="C52" s="0">
-        <v>1021</v>
+        <v>1012</v>
       </c>
       <c r="D52" s="0">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="0">
-        <v>19.139999389648438</v>
+        <v>9.760000228881836</v>
       </c>
       <c r="C53" s="0">
-        <v>1020</v>
+        <v>1028</v>
       </c>
       <c r="D53" s="0">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="0">
-        <v>16.479999542236328</v>
+        <v>22.239999771118164</v>
       </c>
       <c r="C54" s="0">
-        <v>999</v>
+        <v>1010</v>
       </c>
       <c r="D54" s="0">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="0">
-        <v>15.890000343322754</v>
+        <v>28.010000228881836</v>
       </c>
       <c r="C55" s="0">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="D55" s="0">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="0">
-        <v>27.049999237060547</v>
+        <v>11.90999984741211</v>
       </c>
       <c r="C56" s="0">
         <v>1011</v>
       </c>
       <c r="D56" s="0">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" s="0">
-        <v>15.359999656677246</v>
+        <v>16.440000534057617</v>
       </c>
       <c r="C57" s="0">
-        <v>1025</v>
+        <v>1014</v>
       </c>
       <c r="D57" s="0">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="0">
-        <v>23.969999313354492</v>
+        <v>12.529999732971191</v>
       </c>
       <c r="C58" s="0">
-        <v>1022</v>
+        <v>1001</v>
       </c>
       <c r="D58" s="0">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="0">
-        <v>26.3700008392334</v>
+        <v>17.81999969482422</v>
       </c>
       <c r="C59" s="0">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="D59" s="0">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" s="0">
-        <v>20.1299991607666</v>
+        <v>20.530000686645508</v>
       </c>
       <c r="C60" s="0">
-        <v>1020</v>
+        <v>1031</v>
       </c>
       <c r="D60" s="0">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="0">
+        <v>14.430000305175781</v>
+      </c>
+      <c r="C61" s="0">
+        <v>1006</v>
+      </c>
+      <c r="D61" s="0">
         <v>72</v>
       </c>
-      <c r="B61" s="0">
-        <v>16.700000762939453</v>
-      </c>
-      <c r="C61" s="0">
-        <v>1016</v>
-      </c>
-      <c r="D61" s="0">
-        <v>62</v>
-      </c>
       <c r="E61" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="0">
-        <v>10.890000343322754</v>
+        <v>16.540000915527344</v>
       </c>
       <c r="C62" s="0">
-        <v>1026</v>
+        <v>1017</v>
       </c>
       <c r="D62" s="0">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" s="0">
-        <v>9.850000381469727</v>
+        <v>20.56999969482422</v>
       </c>
       <c r="C63" s="0">
-        <v>1025</v>
+        <v>1016</v>
       </c>
       <c r="D63" s="0">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" s="0">
-        <v>7.590000152587891</v>
+        <v>16.75</v>
       </c>
       <c r="C64" s="0">
-        <v>1026</v>
+        <v>1010</v>
       </c>
       <c r="D64" s="0">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="0">
-        <v>36.599998474121094</v>
+        <v>27.43000030517578</v>
       </c>
       <c r="C65" s="0">
-        <v>1007</v>
+        <v>1016</v>
       </c>
       <c r="D65" s="0">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" s="0">
-        <v>12.399999618530273</v>
+        <v>27.190000534057617</v>
       </c>
       <c r="C66" s="0">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="D66" s="0">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="0">
-        <v>19.3799991607666</v>
+        <v>21.149999618530273</v>
       </c>
       <c r="C67" s="0">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D67" s="0">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" s="0">
-        <v>18.049999237060547</v>
+        <v>26.940000534057617</v>
       </c>
       <c r="C68" s="0">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="D68" s="0">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" s="0">
-        <v>16.06999969482422</v>
+        <v>27.850000381469727</v>
       </c>
       <c r="C69" s="0">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="D69" s="0">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>6</v>
@@ -1599,84 +1596,84 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="0">
-        <v>18.1299991607666</v>
+        <v>16.170000076293945</v>
       </c>
       <c r="C70" s="0">
-        <v>1017</v>
+        <v>1009</v>
       </c>
       <c r="D70" s="0">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="0">
-        <v>17.190000534057617</v>
+        <v>19.520000457763672</v>
       </c>
       <c r="C71" s="0">
-        <v>1007</v>
+        <v>1016</v>
       </c>
       <c r="D71" s="0">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B72" s="0">
-        <v>11.039999961853027</v>
+        <v>15.029999732971191</v>
       </c>
       <c r="C72" s="0">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="D72" s="0">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B73" s="0">
-        <v>33.529998779296875</v>
+        <v>13.510000228881836</v>
       </c>
       <c r="C73" s="0">
         <v>1012</v>
       </c>
       <c r="D73" s="0">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" s="0">
-        <v>5.019999980926514</v>
+        <v>34.349998474121094</v>
       </c>
       <c r="C74" s="0">
-        <v>1020</v>
+        <v>1008</v>
       </c>
       <c r="D74" s="0">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>6</v>
@@ -1684,461 +1681,461 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B75" s="0">
-        <v>18.43000030517578</v>
+        <v>15.90999984741211</v>
       </c>
       <c r="C75" s="0">
-        <v>1017</v>
+        <v>1012</v>
       </c>
       <c r="D75" s="0">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" s="0">
-        <v>15.069999694824219</v>
+        <v>17.200000762939453</v>
       </c>
       <c r="C76" s="0">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="D76" s="0">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" s="0">
-        <v>25.420000076293945</v>
+        <v>20.270000457763672</v>
       </c>
       <c r="C77" s="0">
-        <v>1015</v>
+        <v>1034</v>
       </c>
       <c r="D77" s="0">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" s="0">
-        <v>18.110000610351562</v>
+        <v>24.450000762939453</v>
       </c>
       <c r="C78" s="0">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="D78" s="0">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B79" s="0">
-        <v>16.100000381469727</v>
+        <v>23.8700008392334</v>
       </c>
       <c r="C79" s="0">
-        <v>1016</v>
+        <v>1011</v>
       </c>
       <c r="D79" s="0">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" s="0">
-        <v>24.31999969482422</v>
+        <v>17.5</v>
       </c>
       <c r="C80" s="0">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D80" s="0">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B81" s="0">
-        <v>12.600000381469727</v>
+        <v>14.149999618530273</v>
       </c>
       <c r="C81" s="0">
-        <v>1027</v>
+        <v>1012</v>
       </c>
       <c r="D81" s="0">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B82" s="0">
-        <v>17.030000686645508</v>
+        <v>14.020000457763672</v>
       </c>
       <c r="C82" s="0">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D82" s="0">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" s="0">
-        <v>22.950000762939453</v>
+        <v>17.40999984741211</v>
       </c>
       <c r="C83" s="0">
-        <v>1021</v>
+        <v>1009</v>
       </c>
       <c r="D83" s="0">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B84" s="0">
-        <v>18.110000610351562</v>
+        <v>16.959999084472656</v>
       </c>
       <c r="C84" s="0">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="D84" s="0">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B85" s="0">
-        <v>17.6299991607666</v>
+        <v>19.860000610351562</v>
       </c>
       <c r="C85" s="0">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D85" s="0">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" s="0">
-        <v>27.200000762939453</v>
+        <v>17.559999465942383</v>
       </c>
       <c r="C86" s="0">
         <v>1014</v>
       </c>
       <c r="D86" s="0">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B87" s="0">
-        <v>19.040000915527344</v>
+        <v>13.739999771118164</v>
       </c>
       <c r="C87" s="0">
-        <v>1026</v>
+        <v>1007</v>
       </c>
       <c r="D87" s="0">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B88" s="0">
-        <v>5.639999866485596</v>
+        <v>20.079999923706055</v>
       </c>
       <c r="C88" s="0">
         <v>1019</v>
       </c>
       <c r="D88" s="0">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B89" s="0">
-        <v>18.68000030517578</v>
+        <v>28.5</v>
       </c>
       <c r="C89" s="0">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D89" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B90" s="0">
-        <v>25.770000457763672</v>
+        <v>13.300000190734863</v>
       </c>
       <c r="C90" s="0">
-        <v>1018</v>
+        <v>995</v>
       </c>
       <c r="D90" s="0">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B91" s="0">
-        <v>18.75</v>
+        <v>19.799999237060547</v>
       </c>
       <c r="C91" s="0">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="D91" s="0">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92" s="0">
-        <v>17.6299991607666</v>
+        <v>17.299999237060547</v>
       </c>
       <c r="C92" s="0">
-        <v>1015</v>
+        <v>1008</v>
       </c>
       <c r="D92" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B93" s="0">
-        <v>17.75</v>
+        <v>13.399999618530273</v>
       </c>
       <c r="C93" s="0">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="D93" s="0">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B94" s="0">
-        <v>31.170000076293945</v>
+        <v>27.1200008392334</v>
       </c>
       <c r="C94" s="0">
         <v>1013</v>
       </c>
       <c r="D94" s="0">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B95" s="0">
-        <v>16.290000915527344</v>
+        <v>14.069999694824219</v>
       </c>
       <c r="C95" s="0">
-        <v>1024</v>
+        <v>1006</v>
       </c>
       <c r="D95" s="0">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B96" s="0">
-        <v>17.420000076293945</v>
+        <v>26.610000610351562</v>
       </c>
       <c r="C96" s="0">
-        <v>1025</v>
+        <v>1009</v>
       </c>
       <c r="D96" s="0">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B97" s="0">
-        <v>21.690000534057617</v>
+        <v>13.649999618530273</v>
       </c>
       <c r="C97" s="0">
-        <v>997</v>
+        <v>1014</v>
       </c>
       <c r="D97" s="0">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B98" s="0">
-        <v>21.649999618530273</v>
+        <v>17.209999084472656</v>
       </c>
       <c r="C98" s="0">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="D98" s="0">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B99" s="0">
-        <v>18.979999542236328</v>
+        <v>21.989999771118164</v>
       </c>
       <c r="C99" s="0">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D99" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B100" s="0">
-        <v>18.420000076293945</v>
+        <v>11.960000038146973</v>
       </c>
       <c r="C100" s="0">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="D100" s="0">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B101" s="0">
-        <v>18.889999389648438</v>
+        <v>16.899999618530273</v>
       </c>
       <c r="C101" s="0">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="D101" s="0">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>